<commit_message>
Updated master leave list
Highlighted reports that have a corresponding example in light green
</commit_message>
<xml_diff>
--- a/Report Examples/Leave/UBA Leave Reports Oct 2017.xlsx
+++ b/Report Examples/Leave/UBA Leave Reports Oct 2017.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Clients\UBA\Reports\Report Examples\Leave\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tertiusvb\Documents\Visual Studio 2015\Projects\Github\SS_X3_Reports\Report Examples\Leave\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="119">
   <si>
     <t>Priority List</t>
   </si>
@@ -180,9 +180,6 @@
     <t>043</t>
   </si>
   <si>
-    <t>Maternity leave exception report by date for confirmed and unconfirmed staff</t>
-  </si>
-  <si>
     <t>044</t>
   </si>
   <si>
@@ -382,6 +379,12 @@
   </si>
   <si>
     <t>Leave Report List 2017</t>
+  </si>
+  <si>
+    <t>Maternity leave exception report by date for unconfirmed staff</t>
+  </si>
+  <si>
+    <t>Maternity Leave</t>
   </si>
 </sst>
 </file>
@@ -434,7 +437,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -465,8 +468,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -669,12 +678,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -704,9 +724,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -730,9 +747,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -754,6 +768,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2723,32 +2749,32 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R47"/>
+  <dimension ref="A1:R48"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C11" sqref="C11"/>
       <selection pane="topRight" activeCell="C11" sqref="C11"/>
       <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="61.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" style="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="29" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="67.42578125" customWidth="1"/>
     <col min="5" max="5" width="57.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.85546875" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" style="32" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" style="30" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="25.5703125" customWidth="1"/>
     <col min="10" max="10" width="14.85546875" customWidth="1"/>
     <col min="11" max="11" width="20" customWidth="1"/>
     <col min="12" max="12" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="21.5703125" customWidth="1"/>
-    <col min="14" max="14" width="20" style="33" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20" style="31" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16.42578125" customWidth="1"/>
     <col min="16" max="16" width="9.28515625" customWidth="1"/>
     <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
@@ -2756,22 +2782,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
-        <v>117</v>
-      </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="36"/>
+      <c r="A1" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="34"/>
       <c r="Q1" t="s">
         <v>0</v>
       </c>
@@ -2780,20 +2806,20 @@
       </c>
     </row>
     <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="37"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="39"/>
+      <c r="A2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="37"/>
       <c r="Q2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2905,36 +2931,36 @@
       <c r="C6" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16" t="s">
+      <c r="E6" s="15"/>
+      <c r="F6" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="H6" s="16">
+      <c r="G6" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="H6" s="15">
         <v>3</v>
       </c>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="17">
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="16">
         <v>43054</v>
       </c>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="19">
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="18">
         <f t="shared" ref="N6:N47" si="0">IF(M6="",,(IFERROR((K6-M6)*-1,0)))</f>
         <v>0</v>
       </c>
-      <c r="O6" s="20" t="s">
+      <c r="O6" s="19" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="21">
+      <c r="A7" s="20">
         <v>2</v>
       </c>
       <c r="B7" s="13" t="s">
@@ -2943,36 +2969,36 @@
       <c r="C7" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22" t="s">
+      <c r="E7" s="21"/>
+      <c r="F7" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="H7" s="23">
+      <c r="G7" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="H7" s="22">
         <v>1</v>
       </c>
-      <c r="I7" s="23"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="17">
+      <c r="I7" s="22"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="16">
         <v>43054</v>
       </c>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="19">
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O7" s="20" t="s">
+      <c r="O7" s="19" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="21">
+      <c r="A8" s="20">
         <v>3</v>
       </c>
       <c r="B8" s="13" t="s">
@@ -2981,36 +3007,36 @@
       <c r="C8" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22" t="s">
+      <c r="E8" s="21"/>
+      <c r="F8" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="H8" s="23">
+      <c r="G8" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="H8" s="22">
         <v>1</v>
       </c>
-      <c r="I8" s="23"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="17">
+      <c r="I8" s="22"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="16">
         <v>43054</v>
       </c>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="19">
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O8" s="20" t="s">
+      <c r="O8" s="19" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="21">
+      <c r="A9" s="20">
         <v>4</v>
       </c>
       <c r="B9" s="13" t="s">
@@ -3019,36 +3045,36 @@
       <c r="C9" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22" t="s">
+      <c r="E9" s="21"/>
+      <c r="F9" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="H9" s="23">
+      <c r="G9" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="H9" s="22">
         <v>1</v>
       </c>
-      <c r="I9" s="23"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="17">
+      <c r="I9" s="22"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="16">
         <v>43054</v>
       </c>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="19">
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O9" s="20" t="s">
+      <c r="O9" s="19" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="21">
+      <c r="A10" s="20">
         <v>5</v>
       </c>
       <c r="B10" s="13" t="s">
@@ -3057,36 +3083,36 @@
       <c r="C10" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22" t="s">
+      <c r="E10" s="21"/>
+      <c r="F10" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="H10" s="23">
+      <c r="G10" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="H10" s="22">
         <v>1</v>
       </c>
-      <c r="I10" s="23"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="17">
+      <c r="I10" s="22"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="16">
         <v>43054</v>
       </c>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="19">
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O10" s="20" t="s">
+      <c r="O10" s="19" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="21">
+      <c r="A11" s="20">
         <v>6</v>
       </c>
       <c r="B11" s="13" t="s">
@@ -3095,36 +3121,36 @@
       <c r="C11" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22" t="s">
+      <c r="E11" s="21"/>
+      <c r="F11" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H11" s="23">
+      <c r="G11" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H11" s="22">
         <v>2</v>
       </c>
-      <c r="I11" s="23"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="17">
+      <c r="I11" s="22"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="16">
         <v>43054</v>
       </c>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="19">
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O11" s="20" t="s">
+      <c r="O11" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="21">
+      <c r="A12" s="20">
         <v>7</v>
       </c>
       <c r="B12" s="13" t="s">
@@ -3133,36 +3159,36 @@
       <c r="C12" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22" t="s">
+      <c r="E12" s="21"/>
+      <c r="F12" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H12" s="23">
+      <c r="G12" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H12" s="22">
         <v>1</v>
       </c>
-      <c r="I12" s="23"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="17">
+      <c r="I12" s="22"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="16">
         <v>43054</v>
       </c>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="19">
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O12" s="20" t="s">
+      <c r="O12" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="21">
+      <c r="A13" s="20">
         <v>8</v>
       </c>
       <c r="B13" s="13" t="s">
@@ -3171,36 +3197,36 @@
       <c r="C13" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22" t="s">
+      <c r="E13" s="21"/>
+      <c r="F13" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H13" s="23">
+      <c r="G13" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H13" s="22">
         <v>1</v>
       </c>
-      <c r="I13" s="23"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="17">
+      <c r="I13" s="22"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="16">
         <v>43054</v>
       </c>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="19">
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O13" s="20" t="s">
+      <c r="O13" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="21">
+      <c r="A14" s="20">
         <v>9</v>
       </c>
       <c r="B14" s="13" t="s">
@@ -3209,38 +3235,38 @@
       <c r="C14" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="22" t="s">
+      <c r="E14" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="22" t="s">
+      <c r="F14" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H14" s="23">
-        <v>0</v>
-      </c>
-      <c r="I14" s="23"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="17">
+      <c r="G14" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H14" s="22">
+        <v>0</v>
+      </c>
+      <c r="I14" s="22"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="16">
         <v>43054</v>
       </c>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="19">
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O14" s="20" t="s">
+      <c r="O14" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="21">
+      <c r="A15" s="20">
         <v>10</v>
       </c>
       <c r="B15" s="13" t="s">
@@ -3249,36 +3275,36 @@
       <c r="C15" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22" t="s">
+      <c r="E15" s="21"/>
+      <c r="F15" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H15" s="23">
+      <c r="G15" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H15" s="22">
         <v>2</v>
       </c>
-      <c r="I15" s="23"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="17">
+      <c r="I15" s="22"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="16">
         <v>43054</v>
       </c>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="19">
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O15" s="20" t="s">
+      <c r="O15" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="21">
+      <c r="A16" s="20">
         <v>11</v>
       </c>
       <c r="B16" s="13" t="s">
@@ -3287,36 +3313,36 @@
       <c r="C16" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D16" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22" t="s">
+      <c r="E16" s="21"/>
+      <c r="F16" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H16" s="23">
+      <c r="G16" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H16" s="22">
         <v>1</v>
       </c>
-      <c r="I16" s="23"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="17">
+      <c r="I16" s="22"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="16">
         <v>43054</v>
       </c>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="19">
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O16" s="20" t="s">
+      <c r="O16" s="19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="21">
+    <row r="17" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="20">
         <v>12</v>
       </c>
       <c r="B17" s="13" t="s">
@@ -3325,1194 +3351,1199 @@
       <c r="C17" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22" t="s">
+      <c r="D17" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G17" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H17" s="23">
+      <c r="G17" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H17" s="22">
         <v>1</v>
       </c>
-      <c r="I17" s="23"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="17">
+      <c r="I17" s="22"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="16">
         <v>43054</v>
       </c>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="19">
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O17" s="20" t="s">
+      <c r="O17" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="21">
+      <c r="A18" s="20">
         <v>13</v>
       </c>
       <c r="B18" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C18" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22" t="s">
+      <c r="E18" s="21"/>
+      <c r="F18" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G18" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H18" s="23">
+      <c r="G18" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H18" s="22">
         <v>2</v>
       </c>
-      <c r="I18" s="23"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="17">
+      <c r="I18" s="22"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="16">
         <v>43054</v>
       </c>
-      <c r="L18" s="18"/>
-      <c r="M18" s="18"/>
-      <c r="N18" s="19">
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O18" s="20" t="s">
+      <c r="O18" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="21">
+      <c r="A19" s="20">
         <v>14</v>
       </c>
       <c r="B19" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C19" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="D19" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22" t="s">
+      <c r="E19" s="21"/>
+      <c r="F19" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H19" s="23">
+      <c r="G19" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H19" s="22">
         <v>3</v>
       </c>
-      <c r="I19" s="23"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="17">
+      <c r="I19" s="22"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="16">
         <v>43054</v>
       </c>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="19">
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O19" s="20" t="s">
+      <c r="O19" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="21">
+      <c r="A20" s="20">
         <v>15</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C20" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="D20" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22" t="s">
+      <c r="E20" s="21"/>
+      <c r="F20" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G20" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H20" s="23">
+      <c r="G20" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H20" s="22">
         <v>1</v>
       </c>
-      <c r="I20" s="23"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="17">
+      <c r="I20" s="22"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="16">
         <v>43054</v>
       </c>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="19">
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O20" s="20" t="s">
+      <c r="O20" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="21">
+      <c r="A21" s="20">
         <v>16</v>
       </c>
       <c r="B21" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C21" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="E21" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="E21" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="F21" s="22" t="s">
+      <c r="F21" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G21" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H21" s="23">
-        <v>0</v>
-      </c>
-      <c r="I21" s="23"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="17">
+      <c r="G21" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H21" s="22">
+        <v>0</v>
+      </c>
+      <c r="I21" s="22"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="16">
         <v>43054</v>
       </c>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="19">
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O21" s="20" t="s">
+      <c r="O21" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="21">
+      <c r="A22" s="20">
         <v>17</v>
       </c>
       <c r="B22" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C22" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="D22" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22" t="s">
+      <c r="E22" s="21"/>
+      <c r="F22" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G22" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H22" s="23">
+      <c r="G22" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H22" s="22">
         <v>1</v>
       </c>
-      <c r="I22" s="23"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="17">
+      <c r="I22" s="22"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="16">
         <v>43054</v>
       </c>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="19">
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O22" s="20" t="s">
+      <c r="O22" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="21">
+      <c r="A23" s="20">
         <v>18</v>
       </c>
       <c r="B23" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C23" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="D23" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22" t="s">
+      <c r="E23" s="21"/>
+      <c r="F23" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G23" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H23" s="23">
+      <c r="G23" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H23" s="22">
         <v>3</v>
       </c>
-      <c r="I23" s="23"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="17">
+      <c r="I23" s="22"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="16">
         <v>43054</v>
       </c>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="19">
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O23" s="20" t="s">
+      <c r="O23" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="21">
+      <c r="A24" s="20">
         <v>19</v>
       </c>
       <c r="B24" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C24" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="D24" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22" t="s">
+      <c r="E24" s="21"/>
+      <c r="F24" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G24" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H24" s="23">
+      <c r="G24" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H24" s="22">
         <v>2</v>
       </c>
-      <c r="I24" s="23"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="17">
+      <c r="I24" s="22"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="16">
         <v>43054</v>
       </c>
-      <c r="L24" s="18"/>
-      <c r="M24" s="18"/>
-      <c r="N24" s="19">
+      <c r="L24" s="17"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O24" s="20" t="s">
+      <c r="O24" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="21">
+      <c r="A25" s="20">
         <v>20</v>
       </c>
       <c r="B25" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C25" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="D25" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22" t="s">
+      <c r="E25" s="21"/>
+      <c r="F25" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G25" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H25" s="23">
+      <c r="G25" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H25" s="22">
         <v>3</v>
       </c>
-      <c r="I25" s="23"/>
-      <c r="J25" s="22"/>
-      <c r="K25" s="17">
+      <c r="I25" s="22"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="16">
         <v>43054</v>
       </c>
-      <c r="L25" s="18"/>
-      <c r="M25" s="18"/>
-      <c r="N25" s="19">
+      <c r="L25" s="17"/>
+      <c r="M25" s="17"/>
+      <c r="N25" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O25" s="20" t="s">
+      <c r="O25" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="21">
+      <c r="A26" s="20">
         <v>21</v>
       </c>
       <c r="B26" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C26" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="D26" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22" t="s">
+      <c r="E26" s="21"/>
+      <c r="F26" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G26" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H26" s="23">
+      <c r="G26" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H26" s="22">
         <v>3</v>
       </c>
-      <c r="I26" s="23"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="17">
+      <c r="I26" s="22"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="16">
         <v>43054</v>
       </c>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="19">
+      <c r="L26" s="17"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O26" s="20" t="s">
+      <c r="O26" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="21">
+      <c r="A27" s="20">
         <v>22</v>
       </c>
       <c r="B27" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C27" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="D27" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22" t="s">
+      <c r="E27" s="21"/>
+      <c r="F27" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G27" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H27" s="23">
+      <c r="G27" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H27" s="22">
         <v>3</v>
       </c>
-      <c r="I27" s="23"/>
-      <c r="J27" s="22"/>
-      <c r="K27" s="17">
+      <c r="I27" s="22"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="16">
         <v>43054</v>
       </c>
-      <c r="L27" s="18"/>
-      <c r="M27" s="18"/>
-      <c r="N27" s="19">
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O27" s="20" t="s">
+      <c r="O27" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="21">
+      <c r="A28" s="20">
         <v>23</v>
       </c>
       <c r="B28" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C28" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="D28" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22" t="s">
+      <c r="E28" s="21"/>
+      <c r="F28" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G28" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H28" s="23">
+      <c r="G28" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H28" s="22">
         <v>3</v>
       </c>
-      <c r="I28" s="23"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="17">
+      <c r="I28" s="22"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="16">
         <v>43054</v>
       </c>
-      <c r="L28" s="18"/>
-      <c r="M28" s="18"/>
-      <c r="N28" s="19">
+      <c r="L28" s="17"/>
+      <c r="M28" s="17"/>
+      <c r="N28" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O28" s="20" t="s">
+      <c r="O28" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="21">
+      <c r="A29" s="20">
         <v>24</v>
       </c>
       <c r="B29" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C29" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="D29" s="20" t="s">
+      <c r="E29" s="21"/>
+      <c r="F29" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="E29" s="22"/>
-      <c r="F29" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="G29" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H29" s="23">
+      <c r="G29" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H29" s="22">
         <v>3</v>
       </c>
-      <c r="I29" s="23"/>
-      <c r="J29" s="22"/>
-      <c r="K29" s="17">
+      <c r="I29" s="22"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="16">
         <v>43054</v>
       </c>
-      <c r="L29" s="18"/>
-      <c r="M29" s="18"/>
-      <c r="N29" s="19">
+      <c r="L29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O29" s="20" t="s">
+      <c r="O29" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="21">
+      <c r="A30" s="20">
         <v>25</v>
       </c>
       <c r="B30" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C30" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D30" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="D30" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="E30" s="22"/>
-      <c r="F30" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="G30" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H30" s="23">
+      <c r="E30" s="21"/>
+      <c r="F30" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="G30" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H30" s="22">
         <v>3</v>
       </c>
-      <c r="I30" s="23"/>
-      <c r="J30" s="22"/>
-      <c r="K30" s="17">
+      <c r="I30" s="22"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="16">
         <v>43054</v>
       </c>
-      <c r="L30" s="18"/>
-      <c r="M30" s="18"/>
-      <c r="N30" s="19">
+      <c r="L30" s="17"/>
+      <c r="M30" s="17"/>
+      <c r="N30" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O30" s="20" t="s">
+      <c r="O30" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="25">
+      <c r="A31" s="24">
         <v>26</v>
       </c>
       <c r="B31" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C31" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="D31" s="26" t="s">
+      <c r="E31" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="E31" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="F31" s="22" t="s">
+      <c r="F31" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G31" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H31" s="22">
-        <v>0</v>
-      </c>
-      <c r="I31" s="22"/>
-      <c r="J31" s="22"/>
-      <c r="K31" s="17">
+      <c r="G31" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H31" s="21">
+        <v>0</v>
+      </c>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="16">
         <v>43054</v>
       </c>
-      <c r="L31" s="18"/>
-      <c r="M31" s="18"/>
-      <c r="N31" s="19">
+      <c r="L31" s="17"/>
+      <c r="M31" s="17"/>
+      <c r="N31" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O31" s="20" t="s">
+      <c r="O31" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="21">
+      <c r="A32" s="20">
         <v>27</v>
       </c>
       <c r="B32" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C32" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D32" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="D32" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22" t="s">
+      <c r="E32" s="21"/>
+      <c r="F32" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G32" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H32" s="22">
+      <c r="G32" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H32" s="21">
         <v>3</v>
       </c>
-      <c r="I32" s="22"/>
-      <c r="J32" s="22"/>
-      <c r="K32" s="17">
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="16">
         <v>43054</v>
       </c>
-      <c r="L32" s="18"/>
-      <c r="M32" s="18"/>
-      <c r="N32" s="19">
+      <c r="L32" s="17"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O32" s="20" t="s">
+      <c r="O32" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="25">
+      <c r="A33" s="24">
         <v>28</v>
       </c>
       <c r="B33" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C33" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="D33" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="E33" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="F33" s="22" t="s">
+      <c r="E33" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="F33" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G33" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H33" s="22">
-        <v>0</v>
-      </c>
-      <c r="I33" s="22"/>
-      <c r="J33" s="22"/>
-      <c r="K33" s="17">
+      <c r="G33" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H33" s="21">
+        <v>0</v>
+      </c>
+      <c r="I33" s="21"/>
+      <c r="J33" s="21"/>
+      <c r="K33" s="16">
         <v>43054</v>
       </c>
-      <c r="L33" s="18"/>
-      <c r="M33" s="18"/>
-      <c r="N33" s="19">
+      <c r="L33" s="17"/>
+      <c r="M33" s="17"/>
+      <c r="N33" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O33" s="20" t="s">
+      <c r="O33" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="25">
+      <c r="A34" s="24">
         <v>29</v>
       </c>
       <c r="B34" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C34" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D34" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="D34" s="26" t="s">
-        <v>87</v>
-      </c>
-      <c r="E34" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="F34" s="22" t="s">
+      <c r="E34" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="F34" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G34" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H34" s="22">
-        <v>0</v>
-      </c>
-      <c r="I34" s="22"/>
-      <c r="J34" s="22"/>
-      <c r="K34" s="17">
+      <c r="G34" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H34" s="21">
+        <v>0</v>
+      </c>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="16">
         <v>43054</v>
       </c>
-      <c r="L34" s="18"/>
-      <c r="M34" s="18"/>
-      <c r="N34" s="19">
+      <c r="L34" s="17"/>
+      <c r="M34" s="17"/>
+      <c r="N34" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O34" s="20" t="s">
+      <c r="O34" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="21">
+      <c r="A35" s="20">
         <v>30</v>
       </c>
       <c r="B35" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C35" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="D35" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="D35" s="20" t="s">
+      <c r="E35" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="E35" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="F35" s="22" t="s">
+      <c r="F35" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G35" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H35" s="22">
+      <c r="G35" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H35" s="21">
         <v>3</v>
       </c>
-      <c r="I35" s="22"/>
-      <c r="J35" s="22"/>
-      <c r="K35" s="17">
+      <c r="I35" s="21"/>
+      <c r="J35" s="21"/>
+      <c r="K35" s="16">
         <v>43054</v>
       </c>
-      <c r="L35" s="18"/>
-      <c r="M35" s="18"/>
-      <c r="N35" s="19">
+      <c r="L35" s="17"/>
+      <c r="M35" s="17"/>
+      <c r="N35" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O35" s="20" t="s">
+      <c r="O35" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="25">
+      <c r="A36" s="24">
         <v>31</v>
       </c>
       <c r="B36" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C36" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D36" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="D36" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="E36" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="F36" s="22" t="s">
+      <c r="E36" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="F36" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G36" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H36" s="22">
-        <v>0</v>
-      </c>
-      <c r="I36" s="22"/>
-      <c r="J36" s="22"/>
-      <c r="K36" s="17">
+      <c r="G36" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H36" s="21">
+        <v>0</v>
+      </c>
+      <c r="I36" s="21"/>
+      <c r="J36" s="21"/>
+      <c r="K36" s="16">
         <v>43054</v>
       </c>
-      <c r="L36" s="18"/>
-      <c r="M36" s="18"/>
-      <c r="N36" s="19">
+      <c r="L36" s="17"/>
+      <c r="M36" s="17"/>
+      <c r="N36" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O36" s="20" t="s">
+      <c r="O36" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="25">
+      <c r="A37" s="24">
         <v>32</v>
       </c>
       <c r="B37" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C37" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D37" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="D37" s="26" t="s">
-        <v>94</v>
-      </c>
-      <c r="E37" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="F37" s="22" t="s">
+      <c r="E37" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="F37" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G37" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H37" s="22">
-        <v>0</v>
-      </c>
-      <c r="I37" s="22"/>
-      <c r="J37" s="22"/>
-      <c r="K37" s="17">
+      <c r="G37" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H37" s="21">
+        <v>0</v>
+      </c>
+      <c r="I37" s="21"/>
+      <c r="J37" s="21"/>
+      <c r="K37" s="16">
         <v>43054</v>
       </c>
-      <c r="L37" s="18"/>
-      <c r="M37" s="18"/>
-      <c r="N37" s="19">
+      <c r="L37" s="17"/>
+      <c r="M37" s="17"/>
+      <c r="N37" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O37" s="20" t="s">
+      <c r="O37" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="25">
+      <c r="A38" s="24">
         <v>33</v>
       </c>
       <c r="B38" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C38" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D38" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="D38" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="E38" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="F38" s="22" t="s">
+      <c r="E38" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="F38" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G38" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H38" s="22">
-        <v>0</v>
-      </c>
-      <c r="I38" s="22"/>
-      <c r="J38" s="22"/>
-      <c r="K38" s="17">
+      <c r="G38" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H38" s="21">
+        <v>0</v>
+      </c>
+      <c r="I38" s="21"/>
+      <c r="J38" s="21"/>
+      <c r="K38" s="16">
         <v>43054</v>
       </c>
-      <c r="L38" s="18"/>
-      <c r="M38" s="18"/>
-      <c r="N38" s="19">
+      <c r="L38" s="17"/>
+      <c r="M38" s="17"/>
+      <c r="N38" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O38" s="20" t="s">
+      <c r="O38" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="25">
+      <c r="A39" s="24">
         <v>34</v>
       </c>
       <c r="B39" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C39" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D39" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="D39" s="26" t="s">
-        <v>98</v>
-      </c>
-      <c r="E39" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="F39" s="22" t="s">
+      <c r="E39" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="F39" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G39" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H39" s="22">
-        <v>0</v>
-      </c>
-      <c r="I39" s="22"/>
-      <c r="J39" s="22"/>
-      <c r="K39" s="17">
+      <c r="G39" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H39" s="21">
+        <v>0</v>
+      </c>
+      <c r="I39" s="21"/>
+      <c r="J39" s="21"/>
+      <c r="K39" s="16">
         <v>43054</v>
       </c>
-      <c r="L39" s="18"/>
-      <c r="M39" s="18"/>
-      <c r="N39" s="19">
+      <c r="L39" s="17"/>
+      <c r="M39" s="17"/>
+      <c r="N39" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O39" s="20" t="s">
+      <c r="O39" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="25">
+      <c r="A40" s="24">
         <v>35</v>
       </c>
       <c r="B40" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C40" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D40" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="D40" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="E40" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="F40" s="22" t="s">
+      <c r="E40" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="F40" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G40" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H40" s="22">
-        <v>0</v>
-      </c>
-      <c r="I40" s="22"/>
-      <c r="J40" s="22"/>
-      <c r="K40" s="17">
+      <c r="G40" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H40" s="21">
+        <v>0</v>
+      </c>
+      <c r="I40" s="21"/>
+      <c r="J40" s="21"/>
+      <c r="K40" s="16">
         <v>43054</v>
       </c>
-      <c r="L40" s="18"/>
-      <c r="M40" s="18"/>
-      <c r="N40" s="19">
+      <c r="L40" s="17"/>
+      <c r="M40" s="17"/>
+      <c r="N40" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O40" s="20" t="s">
+      <c r="O40" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="25">
+      <c r="A41" s="24">
         <v>36</v>
       </c>
       <c r="B41" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C41" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D41" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="D41" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="E41" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="F41" s="22" t="s">
+      <c r="E41" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="F41" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G41" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H41" s="22">
-        <v>0</v>
-      </c>
-      <c r="I41" s="22"/>
-      <c r="J41" s="22"/>
-      <c r="K41" s="17">
+      <c r="G41" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H41" s="21">
+        <v>0</v>
+      </c>
+      <c r="I41" s="21"/>
+      <c r="J41" s="21"/>
+      <c r="K41" s="16">
         <v>43054</v>
       </c>
-      <c r="L41" s="18"/>
-      <c r="M41" s="18"/>
-      <c r="N41" s="19">
+      <c r="L41" s="17"/>
+      <c r="M41" s="17"/>
+      <c r="N41" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O41" s="20" t="s">
+      <c r="O41" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="21">
+      <c r="A42" s="20">
         <v>37</v>
       </c>
       <c r="B42" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C42" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D42" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="D42" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="E42" s="22"/>
-      <c r="F42" s="22" t="s">
+      <c r="E42" s="21"/>
+      <c r="F42" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G42" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H42" s="22">
+      <c r="G42" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H42" s="21">
         <v>2</v>
       </c>
-      <c r="I42" s="22"/>
-      <c r="J42" s="22"/>
-      <c r="K42" s="17">
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
+      <c r="K42" s="16">
         <v>43054</v>
       </c>
-      <c r="L42" s="18"/>
-      <c r="M42" s="18"/>
-      <c r="N42" s="19">
+      <c r="L42" s="17"/>
+      <c r="M42" s="17"/>
+      <c r="N42" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O42" s="20" t="s">
+      <c r="O42" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="21">
+      <c r="A43" s="20">
         <v>38</v>
       </c>
       <c r="B43" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C43" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D43" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="D43" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="E43" s="22"/>
-      <c r="F43" s="22" t="s">
+      <c r="E43" s="21"/>
+      <c r="F43" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G43" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H43" s="22">
+      <c r="G43" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H43" s="21">
         <v>3</v>
       </c>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
-      <c r="K43" s="17">
+      <c r="I43" s="21"/>
+      <c r="J43" s="21"/>
+      <c r="K43" s="16">
         <v>43054</v>
       </c>
-      <c r="L43" s="18"/>
-      <c r="M43" s="18"/>
-      <c r="N43" s="19">
+      <c r="L43" s="17"/>
+      <c r="M43" s="17"/>
+      <c r="N43" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O43" s="20" t="s">
+      <c r="O43" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="21">
+      <c r="A44" s="20">
         <v>39</v>
       </c>
       <c r="B44" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C44" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="D44" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="D44" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="E44" s="22"/>
-      <c r="F44" s="22" t="s">
+      <c r="E44" s="21"/>
+      <c r="F44" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G44" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H44" s="22">
+      <c r="G44" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H44" s="21">
         <v>1</v>
       </c>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
-      <c r="K44" s="17">
+      <c r="I44" s="21"/>
+      <c r="J44" s="21"/>
+      <c r="K44" s="16">
         <v>43054</v>
       </c>
-      <c r="L44" s="18"/>
-      <c r="M44" s="18"/>
-      <c r="N44" s="19">
+      <c r="L44" s="17"/>
+      <c r="M44" s="17"/>
+      <c r="N44" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O44" s="20" t="s">
+      <c r="O44" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="21">
+      <c r="A45" s="20">
         <v>40</v>
       </c>
       <c r="B45" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C45" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="D45" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="D45" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="E45" s="22"/>
-      <c r="F45" s="22" t="s">
+      <c r="E45" s="21"/>
+      <c r="F45" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G45" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H45" s="22">
+      <c r="G45" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H45" s="21">
         <v>1</v>
       </c>
-      <c r="I45" s="22"/>
-      <c r="J45" s="22"/>
-      <c r="K45" s="17">
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
+      <c r="K45" s="16">
         <v>43054</v>
       </c>
-      <c r="L45" s="18"/>
-      <c r="M45" s="18"/>
-      <c r="N45" s="19">
+      <c r="L45" s="17"/>
+      <c r="M45" s="17"/>
+      <c r="N45" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O45" s="20" t="s">
+      <c r="O45" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="21">
+      <c r="A46" s="20">
         <v>41</v>
       </c>
       <c r="B46" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C46" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="D46" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="D46" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="E46" s="22"/>
-      <c r="F46" s="22" t="s">
+      <c r="E46" s="21"/>
+      <c r="F46" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G46" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H46" s="22">
+      <c r="G46" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H46" s="21">
         <v>2</v>
       </c>
-      <c r="I46" s="22"/>
-      <c r="J46" s="22"/>
-      <c r="K46" s="17">
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
+      <c r="K46" s="16">
         <v>43054</v>
       </c>
-      <c r="L46" s="18"/>
-      <c r="M46" s="18"/>
-      <c r="N46" s="19">
+      <c r="L46" s="17"/>
+      <c r="M46" s="17"/>
+      <c r="N46" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O46" s="20" t="s">
+      <c r="O46" s="19" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="28">
+      <c r="A47" s="27">
         <v>42</v>
       </c>
       <c r="B47" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C47" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D47" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="D47" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="E47" s="30"/>
-      <c r="F47" s="30" t="s">
+      <c r="E47" s="28"/>
+      <c r="F47" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="G47" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="H47" s="30">
+      <c r="G47" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="H47" s="28">
         <v>1</v>
       </c>
-      <c r="I47" s="30"/>
-      <c r="J47" s="30"/>
-      <c r="K47" s="17">
+      <c r="I47" s="28"/>
+      <c r="J47" s="28"/>
+      <c r="K47" s="16">
         <v>43054</v>
       </c>
-      <c r="L47" s="18"/>
-      <c r="M47" s="18"/>
-      <c r="N47" s="19">
+      <c r="L47" s="17"/>
+      <c r="M47" s="17"/>
+      <c r="N47" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O47" s="20" t="s">
+      <c r="O47" s="19" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D48" s="41" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>